<commit_message>
Fetch data from excel file
</commit_message>
<xml_diff>
--- a/src/libro1.xlsx
+++ b/src/libro1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Nan-HDD\Programacion\Projects\39-marathon-app\src\app\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Nan-HDD\Programacion\Projects\39-marathon-app\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -92,7 +92,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -137,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -151,7 +151,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +467,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1079</v>
       </c>
@@ -524,7 +527,7 @@
         <v>38272</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1082</v>
       </c>
@@ -583,6 +586,9 @@
       <c r="F7" s="2">
         <v>38275</v>
       </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change the table head
</commit_message>
<xml_diff>
--- a/src/libro1.xlsx
+++ b/src/libro1.xlsx
@@ -438,7 +438,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,10 +452,10 @@
         <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>

</xml_diff>